<commit_message>
korrektur ip addresses Ergänzung management ip
</commit_message>
<xml_diff>
--- a/Iuk_III_U_addressplann.xlsx
+++ b/Iuk_III_U_addressplann.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
   <si>
     <t>R1</t>
   </si>
@@ -186,18 +186,9 @@
     <t>10.1.40.10</t>
   </si>
   <si>
-    <t>10.1.40.16</t>
-  </si>
-  <si>
     <t>10.1.40.17</t>
   </si>
   <si>
-    <t>10.1.40.24</t>
-  </si>
-  <si>
-    <t>10.1.40.25</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -273,9 +264,6 @@
     <t>2001:620:3101:1043::1/64</t>
   </si>
   <si>
-    <t>Po3</t>
-  </si>
-  <si>
     <t>2001:620:3101:1044::1/64</t>
   </si>
   <si>
@@ -331,6 +319,42 @@
   </si>
   <si>
     <t>g0/22</t>
+  </si>
+  <si>
+    <t>10.1.40.13</t>
+  </si>
+  <si>
+    <t>10.1.40.14</t>
+  </si>
+  <si>
+    <t>10.1.40.18</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>2001:620:3101:1199::1/64</t>
+  </si>
+  <si>
+    <t>10.1.99.10</t>
+  </si>
+  <si>
+    <t>10.1.99.20</t>
+  </si>
+  <si>
+    <t>10.2.99.10</t>
+  </si>
+  <si>
+    <t>2001:620:3101:2199::1/64</t>
+  </si>
+  <si>
+    <t>2001:620:3101:3199::1/64</t>
+  </si>
+  <si>
+    <t>10.3.99.10</t>
+  </si>
+  <si>
+    <t>Po5</t>
   </si>
 </sst>
 </file>
@@ -378,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -401,21 +425,6 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -469,41 +478,36 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
+      <right style="medium">
         <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -808,15 +812,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
@@ -836,11 +841,11 @@
       <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>88</v>
+      <c r="F1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -860,10 +865,10 @@
         <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -881,7 +886,7 @@
         <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -899,7 +904,7 @@
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -919,10 +924,10 @@
         <v>44</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,7 +945,7 @@
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -957,8 +962,8 @@
       <c r="E7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>73</v>
+      <c r="F7" s="12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -975,8 +980,8 @@
       <c r="E8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>74</v>
+      <c r="F8" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -993,8 +998,8 @@
       <c r="E9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>75</v>
+      <c r="F9" s="12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1011,8 +1016,8 @@
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>76</v>
+      <c r="F10" s="12" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1032,10 +1037,10 @@
         <v>44</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,7 +1058,7 @@
         <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1071,7 +1076,7 @@
         <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1089,7 +1094,7 @@
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1107,48 +1112,48 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>81</v>
+      <c r="D16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>81</v>
+      <c r="D17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1166,84 +1171,84 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>84</v>
+      <c r="D21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>84</v>
+      <c r="C22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1261,75 +1266,75 @@
         <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>87</v>
+      <c r="C24" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>87</v>
+      <c r="C25" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>102</v>
+      <c r="B26" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>63</v>
+      <c r="B27" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>44</v>
@@ -1337,8 +1342,8 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="20" t="s">
-        <v>96</v>
+      <c r="B28" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1348,8 +1353,8 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
-      <c r="B29" s="18" t="s">
-        <v>97</v>
+      <c r="B29" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1362,32 +1367,32 @@
       <c r="A30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>63</v>
+      <c r="B31" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>44</v>
@@ -1395,8 +1400,8 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="18" t="s">
-        <v>100</v>
+      <c r="B32" s="15" t="s">
+        <v>96</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -1406,8 +1411,8 @@
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
-      <c r="B33" s="20" t="s">
-        <v>101</v>
+      <c r="B33" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1428,111 +1433,181 @@
       <c r="E34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="1" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="K36" t="s">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="K37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+      <c r="C39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13" t="s">
-        <v>83</v>
-      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
-      <c r="B41" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="16" t="s">
+      <c r="B41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="20" t="s">
-        <v>103</v>
+      <c r="D45" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="16" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>